<commit_message>
hidden columns and rows
</commit_message>
<xml_diff>
--- a/src/Day015_ImageAndOfficeDocumentProcessing/formula.xlsx
+++ b/src/Day015_ImageAndOfficeDocumentProcessing/formula.xlsx
@@ -385,6 +385,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col hidden="1" max="10" min="7" outlineLevel="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="n">
@@ -407,6 +410,17 @@
         </is>
       </c>
     </row>
+    <row hidden="1" outlineLevel="1" r="20"/>
+    <row hidden="1" outlineLevel="1" r="21"/>
+    <row hidden="1" outlineLevel="1" r="22"/>
+    <row hidden="1" outlineLevel="1" r="23"/>
+    <row hidden="1" outlineLevel="1" r="24"/>
+    <row hidden="1" outlineLevel="1" r="25"/>
+    <row hidden="1" outlineLevel="1" r="26"/>
+    <row hidden="1" outlineLevel="1" r="27"/>
+    <row hidden="1" outlineLevel="1" r="28"/>
+    <row hidden="1" outlineLevel="1" r="29"/>
+    <row hidden="1" outlineLevel="1" r="30"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A3:D3"/>

</xml_diff>